<commit_message>
version 2.10.44 - update code use database
</commit_message>
<xml_diff>
--- a/API/src/files/register_assets.xlsx
+++ b/API/src/files/register_assets.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INTS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\REGISTER ASSETS\API\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="437" documentId="13_ncr:1_{A90B752B-B93E-4608-A5D9-64AA50CFD566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AB9418D-5982-4A68-A4D7-199A09948549}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06D5F09-E960-4045-9A54-B659FE05F5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AMA UBS Vila Império I" sheetId="2" r:id="rId1"/>
+    <sheet name="Ativos" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'AMA UBS Vila Império I'!$A$1:$M$100</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Ativos!$A$1:$M$100</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1151,15 +1151,208 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1178,199 +1371,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1715,53 +1715,53 @@
       <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="2.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="2.109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.140625"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.109375"/>
+    <col min="12" max="12" width="15.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33.75" customHeight="1">
-      <c r="A1" s="59"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="63" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="65"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="60"/>
     </row>
     <row r="2" spans="1:15" ht="24.75" customHeight="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="59" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="70" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="65" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="5" t="s">
@@ -1769,18 +1769,18 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="71"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="66"/>
       <c r="M3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1788,131 +1788,131 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="57" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="72">
+      <c r="G4" s="52"/>
+      <c r="H4" s="68">
         <v>45575</v>
       </c>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="74" t="s">
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="75"/>
+      <c r="M4" s="71"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="79" t="s">
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="75"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="71"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="91" t="s">
+      <c r="B6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="75"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="71"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="75"/>
+      <c r="A7" s="81"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="71"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="85"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="79" t="s">
+      <c r="A8" s="81"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="75"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="71"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="85"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="92" t="s">
+      <c r="A9" s="81"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="98" t="s">
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="75"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="88"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="103"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="78"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="74"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
@@ -1924,14 +1924,14 @@
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="57" t="s">
+      <c r="E11" s="52"/>
+      <c r="F11" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1961,14 +1961,14 @@
       <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="40">
         <v>309116</v>
       </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="48" t="s">
+      <c r="E12" s="40"/>
+      <c r="F12" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="49"/>
+      <c r="G12" s="39"/>
       <c r="H12" s="7" t="s">
         <v>30</v>
       </c>
@@ -1998,12 +1998,12 @@
       <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="48" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="49"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
         <v>30</v>
@@ -2025,12 +2025,12 @@
         <v>36</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="48" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="49"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="7" t="s">
         <v>30</v>
       </c>
@@ -2060,12 +2060,12 @@
       <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="48" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="49"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7" t="s">
         <v>30</v>
@@ -2087,12 +2087,12 @@
         <v>36</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="48" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="49"/>
+      <c r="G16" s="39"/>
       <c r="H16" s="7" t="s">
         <v>30</v>
       </c>
@@ -2122,12 +2122,12 @@
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="48" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="49"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7" t="s">
         <v>30</v>
@@ -2149,12 +2149,12 @@
         <v>36</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="48" t="s">
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="49"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="7" t="s">
         <v>30</v>
       </c>
@@ -2184,12 +2184,12 @@
       <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="48" t="s">
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="49"/>
+      <c r="G19" s="39"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7" t="s">
         <v>30</v>
@@ -2211,8 +2211,8 @@
         <v>36</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="8" t="s">
         <v>44</v>
       </c>
@@ -2246,8 +2246,8 @@
       <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="8" t="s">
         <v>45</v>
       </c>
@@ -2273,8 +2273,8 @@
         <v>36</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="8" t="s">
         <v>46</v>
       </c>
@@ -2308,8 +2308,8 @@
       <c r="C23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="49"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="8" t="s">
         <v>47</v>
       </c>
@@ -2335,8 +2335,8 @@
         <v>36</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="8" t="s">
         <v>48</v>
       </c>
@@ -2370,8 +2370,8 @@
       <c r="C25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
       <c r="F25" s="8" t="s">
         <v>49</v>
       </c>
@@ -2432,14 +2432,14 @@
       <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="40">
         <v>2312</v>
       </c>
-      <c r="E27" s="51"/>
-      <c r="F27" s="48" t="s">
+      <c r="E27" s="40"/>
+      <c r="F27" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="49"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7" t="s">
         <v>30</v>
@@ -2463,14 +2463,14 @@
       <c r="C28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="40">
         <v>305955</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="48" t="s">
+      <c r="E28" s="40"/>
+      <c r="F28" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G28" s="49"/>
+      <c r="G28" s="39"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7" t="s">
         <v>30</v>
@@ -2492,12 +2492,12 @@
         <v>36</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="48" t="s">
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="G29" s="49"/>
+      <c r="G29" s="39"/>
       <c r="H29" s="7" t="s">
         <v>30</v>
       </c>
@@ -2527,12 +2527,12 @@
       <c r="C30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="48" t="s">
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="49"/>
+      <c r="G30" s="39"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7" t="s">
         <v>30</v>
@@ -2554,12 +2554,12 @@
         <v>36</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="48" t="s">
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="49"/>
+      <c r="G31" s="39"/>
       <c r="H31" s="7" t="s">
         <v>30</v>
       </c>
@@ -2589,12 +2589,12 @@
       <c r="C32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="48" t="s">
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="49"/>
+      <c r="G32" s="39"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7" t="s">
         <v>30</v>
@@ -2616,12 +2616,12 @@
         <v>36</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="48" t="s">
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="49"/>
+      <c r="G33" s="39"/>
       <c r="H33" s="7" t="s">
         <v>30</v>
       </c>
@@ -2651,12 +2651,12 @@
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="48" t="s">
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="49"/>
+      <c r="G34" s="39"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7" t="s">
         <v>30</v>
@@ -2680,14 +2680,14 @@
       <c r="C35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="51">
+      <c r="D35" s="40">
         <v>2389</v>
       </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="48" t="s">
+      <c r="E35" s="40"/>
+      <c r="F35" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="49"/>
+      <c r="G35" s="39"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7" t="s">
         <v>30</v>
@@ -2711,14 +2711,14 @@
       <c r="C36" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="51" t="s">
+      <c r="D36" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51" t="s">
+      <c r="E36" s="40"/>
+      <c r="F36" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="51"/>
+      <c r="G36" s="40"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7" t="s">
         <v>30</v>
@@ -2742,14 +2742,14 @@
       <c r="C37" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="51" t="s">
+      <c r="D37" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51" t="s">
+      <c r="E37" s="40"/>
+      <c r="F37" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="G37" s="51"/>
+      <c r="G37" s="40"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7" t="s">
         <v>30</v>
@@ -2773,14 +2773,14 @@
       <c r="C38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="D38" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51" t="s">
+      <c r="E38" s="40"/>
+      <c r="F38" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="G38" s="51"/>
+      <c r="G38" s="40"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7" t="s">
         <v>30</v>
@@ -2804,12 +2804,12 @@
       <c r="C39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="48" t="s">
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="49"/>
+      <c r="G39" s="39"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7" t="s">
         <v>30</v>
@@ -2831,12 +2831,12 @@
         <v>36</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="48" t="s">
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="G40" s="49"/>
+      <c r="G40" s="39"/>
       <c r="H40" s="7" t="s">
         <v>30</v>
       </c>
@@ -2866,12 +2866,12 @@
       <c r="C41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="48" t="s">
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="49"/>
+      <c r="G41" s="39"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7" t="s">
         <v>30</v>
@@ -2893,12 +2893,12 @@
         <v>36</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="48" t="s">
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G42" s="49"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="7" t="s">
         <v>30</v>
       </c>
@@ -2928,12 +2928,12 @@
       <c r="C43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="48" t="s">
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="49"/>
+      <c r="G43" s="39"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7" t="s">
         <v>30</v>
@@ -2955,12 +2955,12 @@
         <v>36</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="48" t="s">
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="G44" s="49"/>
+      <c r="G44" s="39"/>
       <c r="H44" s="7" t="s">
         <v>30</v>
       </c>
@@ -2990,14 +2990,14 @@
       <c r="C45" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="51">
+      <c r="D45" s="40">
         <v>2316</v>
       </c>
-      <c r="E45" s="51"/>
-      <c r="F45" s="48" t="s">
+      <c r="E45" s="40"/>
+      <c r="F45" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="G45" s="49"/>
+      <c r="G45" s="39"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7" t="s">
         <v>30</v>
@@ -3019,12 +3019,12 @@
         <v>36</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="54" t="s">
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="G46" s="49"/>
+      <c r="G46" s="39"/>
       <c r="H46" s="7" t="s">
         <v>30</v>
       </c>
@@ -3054,8 +3054,8 @@
       <c r="C47" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
       <c r="F47" s="16" t="s">
         <v>83</v>
       </c>
@@ -3081,8 +3081,8 @@
         <v>36</v>
       </c>
       <c r="C48" s="18"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
       <c r="F48" s="16" t="s">
         <v>82</v>
       </c>
@@ -3116,8 +3116,8 @@
       <c r="C49" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
       <c r="F49" s="16" t="s">
         <v>84</v>
       </c>
@@ -3145,10 +3145,10 @@
       <c r="C50" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D50" s="37">
+      <c r="D50" s="48">
         <v>2334</v>
       </c>
-      <c r="E50" s="38"/>
+      <c r="E50" s="49"/>
       <c r="F50" s="16" t="s">
         <v>86</v>
       </c>
@@ -3174,12 +3174,12 @@
         <v>36</v>
       </c>
       <c r="C51" s="11"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="48" t="s">
+      <c r="D51" s="44"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="G51" s="49"/>
+      <c r="G51" s="39"/>
       <c r="H51" s="7" t="s">
         <v>30</v>
       </c>
@@ -3209,12 +3209,12 @@
       <c r="C52" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="106" t="s">
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="G52" s="49"/>
+      <c r="G52" s="39"/>
       <c r="H52" s="7"/>
       <c r="I52" s="7" t="s">
         <v>30</v>
@@ -3238,10 +3238,10 @@
       <c r="C53" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D53" s="39">
+      <c r="D53" s="102">
         <v>2311</v>
       </c>
-      <c r="E53" s="39"/>
+      <c r="E53" s="102"/>
       <c r="F53" s="21" t="s">
         <v>90</v>
       </c>
@@ -3269,12 +3269,12 @@
       <c r="C54" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="104" t="s">
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="49"/>
+      <c r="G54" s="39"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7" t="s">
         <v>30</v>
@@ -3296,12 +3296,12 @@
         <v>36</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="51"/>
-      <c r="F55" s="48" t="s">
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="G55" s="49"/>
+      <c r="G55" s="39"/>
       <c r="H55" s="7" t="s">
         <v>30</v>
       </c>
@@ -3331,12 +3331,12 @@
       <c r="C56" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="48" t="s">
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="G56" s="49"/>
+      <c r="G56" s="39"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7" t="s">
         <v>30</v>
@@ -3358,12 +3358,12 @@
         <v>36</v>
       </c>
       <c r="C57" s="1"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="48" t="s">
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="G57" s="49"/>
+      <c r="G57" s="39"/>
       <c r="H57" s="7" t="s">
         <v>30</v>
       </c>
@@ -3391,12 +3391,12 @@
         <v>36</v>
       </c>
       <c r="C58" s="15"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="49" t="s">
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="G58" s="51"/>
+      <c r="G58" s="40"/>
       <c r="H58" s="7" t="s">
         <v>30</v>
       </c>
@@ -3426,12 +3426,12 @@
       <c r="C59" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="49" t="s">
+      <c r="D59" s="104"/>
+      <c r="E59" s="104"/>
+      <c r="F59" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="G59" s="51"/>
+      <c r="G59" s="40"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7" t="s">
         <v>30</v>
@@ -3453,12 +3453,12 @@
         <v>36</v>
       </c>
       <c r="C60" s="15"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="107" t="s">
+      <c r="D60" s="102"/>
+      <c r="E60" s="102"/>
+      <c r="F60" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="G60" s="49"/>
+      <c r="G60" s="39"/>
       <c r="H60" s="7" t="s">
         <v>30</v>
       </c>
@@ -3488,12 +3488,12 @@
       <c r="C61" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="107" t="s">
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="G61" s="49"/>
+      <c r="G61" s="39"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7" t="s">
         <v>30</v>
@@ -3515,9 +3515,9 @@
         <v>36</v>
       </c>
       <c r="C62" s="1"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="108" t="s">
+      <c r="D62" s="53"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="37" t="s">
         <v>102</v>
       </c>
       <c r="H62" s="7" t="s">
@@ -3549,12 +3549,12 @@
       <c r="C63" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D63" s="51"/>
-      <c r="E63" s="51"/>
-      <c r="F63" s="48" t="s">
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="G63" s="49"/>
+      <c r="G63" s="39"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7" t="s">
         <v>30</v>
@@ -3578,12 +3578,12 @@
       <c r="C64" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="51"/>
-      <c r="E64" s="51"/>
-      <c r="F64" s="48" t="s">
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G64" s="49"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="7"/>
       <c r="I64" s="7" t="s">
         <v>30</v>
@@ -3605,12 +3605,12 @@
         <v>36</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="48" t="s">
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="G65" s="49"/>
+      <c r="G65" s="39"/>
       <c r="H65" s="7" t="s">
         <v>30</v>
       </c>
@@ -3640,14 +3640,14 @@
       <c r="C66" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D66" s="51">
+      <c r="D66" s="40">
         <v>2209</v>
       </c>
-      <c r="E66" s="51"/>
-      <c r="F66" s="48" t="s">
+      <c r="E66" s="40"/>
+      <c r="F66" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="G66" s="49"/>
+      <c r="G66" s="39"/>
       <c r="H66" s="7"/>
       <c r="I66" s="7" t="s">
         <v>30</v>
@@ -3671,12 +3671,12 @@
       <c r="C67" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D67" s="51"/>
-      <c r="E67" s="51"/>
-      <c r="F67" s="48" t="s">
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="G67" s="49"/>
+      <c r="G67" s="39"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7" t="s">
         <v>30</v>
@@ -3700,12 +3700,12 @@
       <c r="C68" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D68" s="51"/>
-      <c r="E68" s="51"/>
-      <c r="F68" s="48" t="s">
+      <c r="D68" s="40"/>
+      <c r="E68" s="40"/>
+      <c r="F68" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="G68" s="49"/>
+      <c r="G68" s="39"/>
       <c r="H68" s="7" t="s">
         <v>30</v>
       </c>
@@ -3735,14 +3735,14 @@
       <c r="C69" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D69" s="51">
+      <c r="D69" s="40">
         <v>2319</v>
       </c>
-      <c r="E69" s="51"/>
-      <c r="F69" s="48" t="s">
+      <c r="E69" s="40"/>
+      <c r="F69" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="G69" s="49"/>
+      <c r="G69" s="39"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7" t="s">
         <v>30</v>
@@ -3766,8 +3766,8 @@
       <c r="C70" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D70" s="52"/>
-      <c r="E70" s="53"/>
+      <c r="D70" s="100"/>
+      <c r="E70" s="101"/>
       <c r="F70" s="17" t="s">
         <v>117</v>
       </c>
@@ -3793,8 +3793,8 @@
         <v>118</v>
       </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="51"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
       <c r="F71" s="17" t="s">
         <v>119</v>
       </c>
@@ -3828,14 +3828,14 @@
       <c r="C72" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="D72" s="56">
+      <c r="D72" s="43">
         <v>2318</v>
       </c>
-      <c r="E72" s="56"/>
-      <c r="F72" s="54" t="s">
+      <c r="E72" s="43"/>
+      <c r="F72" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="G72" s="55"/>
+      <c r="G72" s="45"/>
       <c r="H72" s="12"/>
       <c r="I72" s="7" t="s">
         <v>30</v>
@@ -3859,8 +3859,8 @@
       <c r="C73" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D73" s="46"/>
-      <c r="E73" s="46"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
       <c r="F73" s="16" t="s">
         <v>121</v>
       </c>
@@ -3886,8 +3886,8 @@
         <v>118</v>
       </c>
       <c r="C74" s="18"/>
-      <c r="D74" s="46"/>
-      <c r="E74" s="46"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
       <c r="F74" s="16" t="s">
         <v>122</v>
       </c>
@@ -3921,14 +3921,14 @@
       <c r="C75" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D75" s="37">
+      <c r="D75" s="48">
         <v>2313</v>
       </c>
-      <c r="E75" s="38"/>
-      <c r="F75" s="46" t="s">
+      <c r="E75" s="49"/>
+      <c r="F75" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="G75" s="46"/>
+      <c r="G75" s="41"/>
       <c r="H75" s="14"/>
       <c r="I75" s="7" t="s">
         <v>30</v>
@@ -3950,12 +3950,12 @@
         <v>36</v>
       </c>
       <c r="C76" s="19"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="104" t="s">
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="G76" s="105"/>
+      <c r="G76" s="103"/>
       <c r="H76" s="7" t="s">
         <v>30</v>
       </c>
@@ -3983,14 +3983,14 @@
         <v>51</v>
       </c>
       <c r="C77" s="1"/>
-      <c r="D77" s="51">
+      <c r="D77" s="40">
         <v>2354</v>
       </c>
-      <c r="E77" s="51"/>
-      <c r="F77" s="48" t="s">
+      <c r="E77" s="40"/>
+      <c r="F77" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="G77" s="49"/>
+      <c r="G77" s="39"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7" t="s">
         <v>30</v>
@@ -4014,12 +4014,12 @@
       <c r="C78" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D78" s="51"/>
-      <c r="E78" s="51"/>
-      <c r="F78" s="48" t="s">
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
+      <c r="F78" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="G78" s="49"/>
+      <c r="G78" s="39"/>
       <c r="H78" s="7"/>
       <c r="I78" s="7" t="s">
         <v>30</v>
@@ -4041,8 +4041,8 @@
         <v>36</v>
       </c>
       <c r="C79" s="1"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="49"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="39"/>
       <c r="F79" s="8" t="s">
         <v>130</v>
       </c>
@@ -4076,8 +4076,8 @@
       <c r="C80" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D80" s="48"/>
-      <c r="E80" s="49"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="39"/>
       <c r="F80" s="8" t="s">
         <v>131</v>
       </c>
@@ -4103,8 +4103,8 @@
         <v>36</v>
       </c>
       <c r="C81" s="1"/>
-      <c r="D81" s="48"/>
-      <c r="E81" s="49"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="39"/>
       <c r="F81" s="8" t="s">
         <v>133</v>
       </c>
@@ -4138,8 +4138,8 @@
       <c r="C82" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D82" s="48"/>
-      <c r="E82" s="49"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="39"/>
       <c r="F82" s="8" t="s">
         <v>134</v>
       </c>
@@ -4167,10 +4167,10 @@
       <c r="C83" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F83" s="48" t="s">
+      <c r="F83" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="G83" s="49"/>
+      <c r="G83" s="39"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7" t="s">
         <v>30</v>
@@ -4192,8 +4192,8 @@
         <v>36</v>
       </c>
       <c r="C84" s="1"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="49"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="39"/>
       <c r="F84" s="8" t="s">
         <v>137</v>
       </c>
@@ -4227,8 +4227,8 @@
       <c r="C85" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D85" s="48"/>
-      <c r="E85" s="49"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="39"/>
       <c r="F85" s="8" t="s">
         <v>138</v>
       </c>
@@ -4256,10 +4256,10 @@
       <c r="C86" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D86" s="48">
+      <c r="D86" s="38">
         <v>2390</v>
       </c>
-      <c r="E86" s="49"/>
+      <c r="E86" s="39"/>
       <c r="F86" s="8" t="s">
         <v>139</v>
       </c>
@@ -4351,10 +4351,10 @@
       <c r="C89" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D89" s="48">
+      <c r="D89" s="38">
         <v>1589</v>
       </c>
-      <c r="E89" s="49"/>
+      <c r="E89" s="39"/>
       <c r="F89" s="8" t="s">
         <v>144</v>
       </c>
@@ -4566,12 +4566,12 @@
         <v>36</v>
       </c>
       <c r="C96" s="1"/>
-      <c r="D96" s="51"/>
-      <c r="E96" s="51"/>
-      <c r="F96" s="48" t="s">
+      <c r="D96" s="40"/>
+      <c r="E96" s="40"/>
+      <c r="F96" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="G96" s="49"/>
+      <c r="G96" s="39"/>
       <c r="H96" s="7" t="s">
         <v>30</v>
       </c>
@@ -4599,14 +4599,14 @@
       <c r="C97" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D97" s="51">
+      <c r="D97" s="40">
         <v>2315</v>
       </c>
-      <c r="E97" s="51"/>
-      <c r="F97" s="48" t="s">
+      <c r="E97" s="40"/>
+      <c r="F97" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="G97" s="49"/>
+      <c r="G97" s="39"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7" t="s">
         <v>30</v>
@@ -4630,12 +4630,12 @@
       <c r="C98" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D98" s="51"/>
-      <c r="E98" s="51"/>
-      <c r="F98" s="109" t="s">
+      <c r="D98" s="40"/>
+      <c r="E98" s="40"/>
+      <c r="F98" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="G98" s="49"/>
+      <c r="G98" s="39"/>
       <c r="H98" s="7"/>
       <c r="I98" s="7" t="s">
         <v>30</v>
@@ -4657,12 +4657,12 @@
         <v>36</v>
       </c>
       <c r="C99" s="1"/>
-      <c r="D99" s="51"/>
-      <c r="E99" s="51"/>
-      <c r="F99" s="54" t="s">
+      <c r="D99" s="40"/>
+      <c r="E99" s="40"/>
+      <c r="F99" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="G99" s="55"/>
+      <c r="G99" s="45"/>
       <c r="H99" s="7" t="s">
         <v>30</v>
       </c>
@@ -4692,12 +4692,12 @@
       <c r="C100" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D100" s="56"/>
-      <c r="E100" s="54"/>
-      <c r="F100" s="46" t="s">
+      <c r="D100" s="43"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="G100" s="46"/>
+      <c r="G100" s="41"/>
       <c r="H100" s="14"/>
       <c r="I100" s="7" t="s">
         <v>30</v>
@@ -4719,8 +4719,8 @@
         <v>36</v>
       </c>
       <c r="C101" s="22"/>
-      <c r="D101" s="40"/>
-      <c r="E101" s="41"/>
+      <c r="D101" s="105"/>
+      <c r="E101" s="106"/>
       <c r="F101" s="28" t="s">
         <v>160</v>
       </c>
@@ -4754,8 +4754,8 @@
       <c r="C102" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D102" s="42"/>
-      <c r="E102" s="43"/>
+      <c r="D102" s="107"/>
+      <c r="E102" s="108"/>
       <c r="F102" s="32" t="s">
         <v>161</v>
       </c>
@@ -4783,10 +4783,10 @@
       <c r="C103" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D103" s="39">
+      <c r="D103" s="102">
         <v>2314</v>
       </c>
-      <c r="E103" s="39"/>
+      <c r="E103" s="102"/>
       <c r="F103" s="16" t="s">
         <v>162</v>
       </c>
@@ -4808,8 +4808,8 @@
       <c r="A104" s="18"/>
       <c r="B104" s="18"/>
       <c r="C104" s="31"/>
-      <c r="D104" s="39"/>
-      <c r="E104" s="39"/>
+      <c r="D104" s="102"/>
+      <c r="E104" s="102"/>
       <c r="F104" s="16"/>
       <c r="G104" s="35"/>
       <c r="H104" s="18"/>
@@ -4823,8 +4823,8 @@
       <c r="A105" s="18"/>
       <c r="B105" s="18"/>
       <c r="C105" s="31"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="39"/>
+      <c r="D105" s="102"/>
+      <c r="E105" s="102"/>
       <c r="F105" s="16"/>
       <c r="G105" s="35"/>
       <c r="H105" s="18"/>
@@ -4838,8 +4838,8 @@
       <c r="A106" s="18"/>
       <c r="B106" s="18"/>
       <c r="C106" s="18"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="45"/>
+      <c r="D106" s="109"/>
+      <c r="E106" s="110"/>
       <c r="F106" s="36"/>
       <c r="G106" s="18"/>
       <c r="H106" s="18"/>
@@ -4853,8 +4853,8 @@
       <c r="A107" s="18"/>
       <c r="B107" s="18"/>
       <c r="C107" s="18"/>
-      <c r="D107" s="37"/>
-      <c r="E107" s="38"/>
+      <c r="D107" s="48"/>
+      <c r="E107" s="49"/>
       <c r="F107" s="16"/>
       <c r="G107" s="18"/>
       <c r="H107" s="18"/>
@@ -4868,8 +4868,8 @@
       <c r="A108" s="18"/>
       <c r="B108" s="18"/>
       <c r="C108" s="18"/>
-      <c r="D108" s="37"/>
-      <c r="E108" s="38"/>
+      <c r="D108" s="48"/>
+      <c r="E108" s="49"/>
       <c r="F108" s="16"/>
       <c r="G108" s="18"/>
       <c r="H108" s="18"/>
@@ -4883,8 +4883,8 @@
       <c r="A109" s="18"/>
       <c r="B109" s="18"/>
       <c r="C109" s="18"/>
-      <c r="D109" s="37"/>
-      <c r="E109" s="38"/>
+      <c r="D109" s="48"/>
+      <c r="E109" s="49"/>
       <c r="F109" s="16"/>
       <c r="G109" s="18"/>
       <c r="H109" s="18"/>
@@ -4898,8 +4898,8 @@
       <c r="A110" s="18"/>
       <c r="B110" s="18"/>
       <c r="C110" s="18"/>
-      <c r="D110" s="37"/>
-      <c r="E110" s="38"/>
+      <c r="D110" s="48"/>
+      <c r="E110" s="49"/>
       <c r="F110" s="16"/>
       <c r="G110" s="18"/>
       <c r="H110" s="18"/>
@@ -4913,8 +4913,8 @@
       <c r="A111" s="18"/>
       <c r="B111" s="18"/>
       <c r="C111" s="18"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="38"/>
+      <c r="D111" s="48"/>
+      <c r="E111" s="49"/>
       <c r="F111" s="16"/>
       <c r="G111" s="18"/>
       <c r="H111" s="18"/>
@@ -4949,38 +4949,113 @@
     </row>
   </sheetData>
   <mergeCells count="164">
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:M10"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="A6:C10"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="D7:K7"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="H9:K10"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
@@ -5005,114 +5080,39 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:M10"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="A6:C10"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="H9:K10"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="D37:E37"/>
     <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="F97:G97"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D36:E36"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>